<commit_message>
Add unit tests and refactor
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josef\source\repos\Utilities\Utilities\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josef\source\repos\Utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B9741AC-3795-4CBF-A83A-A99F50319A28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC5F42B8-BA34-4018-9F88-5577A4BA2861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,60 +25,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>serviceName</t>
-  </si>
-  <si>
-    <t>input</t>
-  </si>
-  <si>
-    <t>third party services</t>
-  </si>
-  <si>
-    <t>output</t>
-  </si>
-  <si>
-    <t>ServiceA</t>
-  </si>
-  <si>
-    <t>data1</t>
-  </si>
-  <si>
-    <t>result1</t>
-  </si>
-  <si>
-    <t>ServiceB</t>
-  </si>
-  <si>
-    <t>data2</t>
-  </si>
-  <si>
-    <t>result2</t>
-  </si>
-  <si>
-    <t>ServiceC</t>
-  </si>
-  <si>
-    <t>data3</t>
-  </si>
-  <si>
-    <t>result3</t>
-  </si>
-  <si>
-    <t>ServiceX
-ServiceY</t>
-  </si>
-  <si>
-    <t>ServiceY
-ServiceZ</t>
-  </si>
-  <si>
-    <t>ServiceX
-ServiceZ</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>CarModel</t>
+  </si>
+  <si>
+    <t>LicensePlate</t>
+  </si>
+  <si>
+    <t>ManufacturingYear</t>
+  </si>
+  <si>
+    <t>Features</t>
+  </si>
+  <si>
+    <t>CarModelA</t>
+  </si>
+  <si>
+    <t>LicensePlate1</t>
+  </si>
+  <si>
+    <t>CarModelB</t>
+  </si>
+  <si>
+    <t>LicensePlate2</t>
+  </si>
+  <si>
+    <t>CarModelC</t>
+  </si>
+  <si>
+    <t>LicensePlate3</t>
+  </si>
+  <si>
+    <t>AirConditioning
+PowerSteering</t>
+  </si>
+  <si>
+    <t>PowerSteering
+BucketSeats</t>
+  </si>
+  <si>
+    <t>AirConditioning
+BucketSeats</t>
   </si>
 </sst>
 </file>
@@ -402,10 +393,17 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -434,11 +432,11 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
+      <c r="D2" s="1">
+        <v>1985</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -446,16 +444,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
+      <c r="D3" s="1">
+        <v>1995</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -463,19 +461,20 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>1992</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>